<commit_message>
update and add image
</commit_message>
<xml_diff>
--- a/cluster_center_data.xlsx
+++ b/cluster_center_data.xlsx
@@ -875,199 +875,199 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03</v>
+        <v>0.007</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001</v>
+        <v>-0.001</v>
       </c>
       <c r="E2" t="n">
-        <v>1.381</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>0.173</v>
+        <v>0.063</v>
       </c>
       <c r="G2" t="n">
-        <v>0.004</v>
+        <v>-0.001</v>
       </c>
       <c r="H2" t="n">
-        <v>0.047</v>
+        <v>-0.006</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>1.988</v>
+        <v>3.197</v>
       </c>
       <c r="L2" t="n">
-        <v>0.195</v>
+        <v>0.082</v>
       </c>
       <c r="M2" t="n">
-        <v>0.285</v>
+        <v>0.06</v>
       </c>
       <c r="N2" t="n">
-        <v>0.057</v>
+        <v>-0.011</v>
       </c>
       <c r="O2" t="n">
         <v>0</v>
       </c>
       <c r="P2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Q2" t="n">
         <v>0.001</v>
       </c>
       <c r="R2" t="n">
-        <v>0.043</v>
+        <v>0.025</v>
       </c>
       <c r="S2" t="n">
-        <v>0.201</v>
+        <v>0.347</v>
       </c>
       <c r="T2" t="n">
-        <v>0.001</v>
+        <v>-0.001</v>
       </c>
       <c r="U2" t="n">
         <v>0.015</v>
       </c>
       <c r="V2" t="n">
-        <v>0.28</v>
+        <v>0.178</v>
       </c>
       <c r="W2" t="n">
-        <v>0.382</v>
+        <v>0.136</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.144</v>
+        <v>0.098</v>
       </c>
       <c r="Z2" t="n">
         <v>0</v>
       </c>
       <c r="AA2" t="n">
-        <v>5.845</v>
+        <v>9.842000000000001</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.867</v>
+        <v>0.677</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.136</v>
+        <v>0.012</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
       </c>
       <c r="AE2" t="n">
-        <v>9.430999999999999</v>
+        <v>9.042999999999999</v>
       </c>
       <c r="AF2" t="n">
-        <v>6.271</v>
+        <v>1.604</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.057</v>
+        <v>0.027</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="AI2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AJ2" t="n">
         <v>0.001</v>
       </c>
       <c r="AK2" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.023</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>0.821</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>-0.07199999999999999</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>26.709</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>-0.013</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>-0.011</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>15.932</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>29.992</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>4.546</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.968</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>3.468</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>-0.05</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.061</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>-0.052</v>
+      </c>
+      <c r="BM2" t="n">
         <v>0.005</v>
       </c>
-      <c r="AL2" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.038</v>
-      </c>
-      <c r="AO2" t="n">
-        <v>0.037</v>
-      </c>
-      <c r="AP2" t="n">
-        <v>1.005</v>
-      </c>
-      <c r="AQ2" t="n">
-        <v>0.016</v>
-      </c>
-      <c r="AR2" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AS2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0.159</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>23.411</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0.155</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>0.057</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>18.678</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0.137</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.285</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>25.697</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>3.171</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>2.177</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="BI2" t="n">
-        <v>2.028</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0.572</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0.004</v>
-      </c>
       <c r="BN2" t="n">
-        <v>1.005</v>
+        <v>0.821</v>
       </c>
       <c r="BO2" t="n">
         <v>0</v>
@@ -1076,7 +1076,7 @@
         <v>0</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.113</v>
+        <v>0.036</v>
       </c>
       <c r="BR2" t="n">
         <v>0</v>
@@ -1085,40 +1085,40 @@
         <v>0</v>
       </c>
       <c r="BT2" t="n">
-        <v>0.115</v>
+        <v>-0.068</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.197</v>
+        <v>0.007</v>
       </c>
       <c r="BV2" t="n">
-        <v>0.024</v>
+        <v>-0.007</v>
       </c>
       <c r="BW2" t="n">
-        <v>0.03</v>
+        <v>0.007</v>
       </c>
       <c r="BX2" t="n">
-        <v>0.047</v>
+        <v>-0.006</v>
       </c>
       <c r="BY2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BZ2" t="n">
-        <v>0.031</v>
+        <v>0.005</v>
       </c>
       <c r="CA2" t="n">
-        <v>0.195</v>
+        <v>0.082</v>
       </c>
       <c r="CB2" t="n">
         <v>0</v>
       </c>
       <c r="CC2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CD2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CE2" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CF2" t="n">
         <v>-0</v>
@@ -1127,13 +1127,13 @@
         <v>0</v>
       </c>
       <c r="CH2" t="n">
-        <v>1.341</v>
+        <v>0.455</v>
       </c>
       <c r="CI2" t="n">
-        <v>1.877</v>
+        <v>1.817</v>
       </c>
       <c r="CJ2" t="n">
-        <v>356.909</v>
+        <v>307.586</v>
       </c>
     </row>
     <row r="3">
@@ -1141,25 +1141,25 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.057</v>
+        <v>0.043</v>
       </c>
       <c r="C3" t="n">
         <v>0.003</v>
       </c>
       <c r="D3" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="E3" t="n">
-        <v>1.011</v>
+        <v>0.608</v>
       </c>
       <c r="F3" t="n">
-        <v>0.194</v>
+        <v>0.145</v>
       </c>
       <c r="G3" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>0.101</v>
+        <v>0.093</v>
       </c>
       <c r="I3" t="n">
         <v>-0</v>
@@ -1168,19 +1168,19 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>1.923</v>
+        <v>2.184</v>
       </c>
       <c r="L3" t="n">
-        <v>0.144</v>
+        <v>0.191</v>
       </c>
       <c r="M3" t="n">
-        <v>0.548</v>
+        <v>0.457</v>
       </c>
       <c r="N3" t="n">
-        <v>0.116</v>
+        <v>0.106</v>
       </c>
       <c r="O3" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="P3" t="n">
         <v>0</v>
@@ -1189,52 +1189,52 @@
         <v>0.001</v>
       </c>
       <c r="R3" t="n">
-        <v>0.075</v>
+        <v>0.06900000000000001</v>
       </c>
       <c r="S3" t="n">
-        <v>0.093</v>
+        <v>0.243</v>
       </c>
       <c r="T3" t="n">
         <v>0.007</v>
       </c>
       <c r="U3" t="n">
-        <v>0.023</v>
+        <v>0.026</v>
       </c>
       <c r="V3" t="n">
-        <v>0.345</v>
+        <v>0.373</v>
       </c>
       <c r="W3" t="n">
-        <v>0.553</v>
+        <v>0.575</v>
       </c>
       <c r="X3" t="n">
         <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.188</v>
+        <v>0.203</v>
       </c>
       <c r="Z3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.348</v>
+        <v>3.038</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.03</v>
+        <v>0.945</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.173</v>
+        <v>0.141</v>
       </c>
       <c r="AD3" t="n">
         <v>-0</v>
       </c>
       <c r="AE3" t="n">
-        <v>1.257</v>
+        <v>4.949</v>
       </c>
       <c r="AF3" t="n">
-        <v>3.629</v>
+        <v>0.358</v>
       </c>
       <c r="AG3" t="n">
-        <v>0.033</v>
+        <v>0.048</v>
       </c>
       <c r="AH3" t="n">
         <v>0.012</v>
@@ -1246,7 +1246,7 @@
         <v>0.002</v>
       </c>
       <c r="AK3" t="n">
-        <v>0.017</v>
+        <v>0.013</v>
       </c>
       <c r="AL3" t="n">
         <v>0</v>
@@ -1255,16 +1255,16 @@
         <v>0</v>
       </c>
       <c r="AN3" t="n">
-        <v>0.043</v>
+        <v>0.048</v>
       </c>
       <c r="AO3" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.057</v>
       </c>
       <c r="AP3" t="n">
-        <v>0.202</v>
+        <v>0.645</v>
       </c>
       <c r="AQ3" t="n">
-        <v>0.032</v>
+        <v>0.027</v>
       </c>
       <c r="AR3" t="n">
         <v>0</v>
@@ -1273,67 +1273,67 @@
         <v>0</v>
       </c>
       <c r="AT3" t="n">
-        <v>0.243</v>
+        <v>0.194</v>
       </c>
       <c r="AU3" t="n">
-        <v>0.147</v>
+        <v>0.142</v>
       </c>
       <c r="AV3" t="n">
-        <v>4.042</v>
+        <v>9.709</v>
       </c>
       <c r="AW3" t="n">
-        <v>0.23</v>
+        <v>0.15</v>
       </c>
       <c r="AX3" t="n">
         <v>0.001</v>
       </c>
       <c r="AY3" t="n">
-        <v>0.116</v>
+        <v>0.106</v>
       </c>
       <c r="AZ3" t="n">
-        <v>6.107</v>
+        <v>7.772</v>
       </c>
       <c r="BA3" t="n">
-        <v>0.243</v>
+        <v>0.195</v>
       </c>
       <c r="BB3" t="n">
-        <v>0.548</v>
+        <v>0.457</v>
       </c>
       <c r="BC3" t="n">
-        <v>6.384</v>
+        <v>12.247</v>
       </c>
       <c r="BD3" t="n">
         <v>0.008999999999999999</v>
       </c>
       <c r="BE3" t="n">
-        <v>1.574</v>
+        <v>2.579</v>
       </c>
       <c r="BF3" t="n">
-        <v>1.382</v>
+        <v>1.555</v>
       </c>
       <c r="BG3" t="n">
         <v>0.003</v>
       </c>
       <c r="BH3" t="n">
-        <v>0.51</v>
+        <v>0.543</v>
       </c>
       <c r="BI3" t="n">
-        <v>0.409</v>
+        <v>1.22</v>
       </c>
       <c r="BJ3" t="n">
-        <v>0.551</v>
+        <v>0.424</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.225</v>
+        <v>0.08699999999999999</v>
       </c>
       <c r="BL3" t="n">
-        <v>0.013</v>
+        <v>0.019</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.022</v>
+        <v>0.019</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.202</v>
+        <v>0.645</v>
       </c>
       <c r="BO3" t="n">
         <v>0</v>
@@ -1342,7 +1342,7 @@
         <v>0</v>
       </c>
       <c r="BQ3" t="n">
-        <v>0.201</v>
+        <v>0.199</v>
       </c>
       <c r="BR3" t="n">
         <v>0</v>
@@ -1351,28 +1351,28 @@
         <v>0</v>
       </c>
       <c r="BT3" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="BU3" t="n">
         <v>0.31</v>
       </c>
-      <c r="BU3" t="n">
-        <v>0.368</v>
-      </c>
       <c r="BV3" t="n">
-        <v>0.029</v>
+        <v>0.026</v>
       </c>
       <c r="BW3" t="n">
-        <v>0.055</v>
+        <v>0.042</v>
       </c>
       <c r="BX3" t="n">
-        <v>0.101</v>
+        <v>0.093</v>
       </c>
       <c r="BY3" t="n">
         <v>0</v>
       </c>
       <c r="BZ3" t="n">
-        <v>0.057</v>
+        <v>0.048</v>
       </c>
       <c r="CA3" t="n">
-        <v>0.144</v>
+        <v>0.191</v>
       </c>
       <c r="CB3" t="n">
         <v>0.002</v>
@@ -1387,19 +1387,19 @@
         <v>0</v>
       </c>
       <c r="CF3" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="CG3" t="n">
         <v>0</v>
       </c>
       <c r="CH3" t="n">
-        <v>0.962</v>
+        <v>0.384</v>
       </c>
       <c r="CI3" t="n">
-        <v>0.074</v>
+        <v>0.971</v>
       </c>
       <c r="CJ3" t="n">
-        <v>169.801</v>
+        <v>209.485</v>
       </c>
     </row>
     <row r="4">
@@ -1407,112 +1407,112 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.004</v>
+        <v>-0.03</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.002</v>
+        <v>-0.001</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.002</v>
+        <v>-0</v>
       </c>
       <c r="E4" t="n">
-        <v>1.558</v>
+        <v>2.77</v>
       </c>
       <c r="F4" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.003</v>
+        <v>-0.007</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.006</v>
+        <v>0.083</v>
       </c>
       <c r="I4" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="J4" t="n">
         <v>-0</v>
       </c>
       <c r="K4" t="n">
-        <v>2.147</v>
+        <v>0.749</v>
       </c>
       <c r="L4" t="n">
-        <v>0.185</v>
+        <v>0.08</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.031</v>
+        <v>-0.213</v>
       </c>
       <c r="N4" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-0.018</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.059</v>
+      </c>
+      <c r="T4" t="n">
+        <v>-0</v>
+      </c>
+      <c r="U4" t="n">
         <v>-0.02</v>
       </c>
-      <c r="O4" t="n">
-        <v>0</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="R4" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="S4" t="n">
-        <v>0.254</v>
-      </c>
-      <c r="T4" t="n">
-        <v>-0.004</v>
-      </c>
-      <c r="U4" t="n">
-        <v>0.003</v>
-      </c>
       <c r="V4" t="n">
-        <v>0.159</v>
+        <v>-0.046</v>
       </c>
       <c r="W4" t="n">
-        <v>0.155</v>
+        <v>0.11</v>
       </c>
       <c r="X4" t="n">
         <v>-0</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.075</v>
+        <v>-0.028</v>
       </c>
       <c r="Z4" t="n">
         <v>0</v>
       </c>
       <c r="AA4" t="n">
-        <v>10.156</v>
+        <v>4.526</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.5629999999999999</v>
+        <v>-0.249</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.049</v>
+        <v>-0.018</v>
       </c>
       <c r="AD4" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="AE4" t="n">
-        <v>16.684</v>
+        <v>24.051</v>
       </c>
       <c r="AF4" t="n">
-        <v>6.863</v>
+        <v>0.426</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.058</v>
+        <v>0.006</v>
       </c>
       <c r="AH4" t="n">
-        <v>-0.004</v>
+        <v>-0.008</v>
       </c>
       <c r="AI4" t="n">
         <v>-0</v>
       </c>
       <c r="AJ4" t="n">
-        <v>-0</v>
+        <v>-0.001</v>
       </c>
       <c r="AK4" t="n">
-        <v>-0.003</v>
+        <v>0.006</v>
       </c>
       <c r="AL4" t="n">
         <v>-0</v>
@@ -1521,85 +1521,85 @@
         <v>-0</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="AO4" t="n">
-        <v>-0.005</v>
+        <v>-0.021</v>
       </c>
       <c r="AP4" t="n">
-        <v>1.485</v>
+        <v>1.77</v>
       </c>
       <c r="AQ4" t="n">
-        <v>-0.006</v>
+        <v>-0.021</v>
       </c>
       <c r="AR4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AS4" t="n">
         <v>-0</v>
       </c>
       <c r="AT4" t="n">
-        <v>-0.004</v>
+        <v>-0.134</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.12</v>
+        <v>0.37</v>
       </c>
       <c r="AV4" t="n">
-        <v>40.272</v>
+        <v>40.298</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.1</v>
+        <v>0.343</v>
       </c>
       <c r="AX4" t="n">
         <v>-0.001</v>
       </c>
       <c r="AY4" t="n">
-        <v>-0.02</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="AZ4" t="n">
-        <v>27.902</v>
+        <v>25.528</v>
       </c>
       <c r="BA4" t="n">
-        <v>-0.005</v>
+        <v>-0.134</v>
       </c>
       <c r="BB4" t="n">
-        <v>-0.032</v>
+        <v>-0.213</v>
       </c>
       <c r="BC4" t="n">
-        <v>42.593</v>
+        <v>41.361</v>
       </c>
       <c r="BD4" t="n">
-        <v>-0.003</v>
+        <v>-0.007</v>
       </c>
       <c r="BE4" t="n">
-        <v>4.222</v>
+        <v>1.538</v>
       </c>
       <c r="BF4" t="n">
-        <v>2.483</v>
+        <v>3.423</v>
       </c>
       <c r="BG4" t="n">
         <v>-0.001</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.18</v>
+        <v>0.005</v>
       </c>
       <c r="BI4" t="n">
-        <v>3.356</v>
+        <v>1.537</v>
       </c>
       <c r="BJ4" t="n">
-        <v>-0.046</v>
+        <v>0.4</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.801</v>
+        <v>1.18</v>
       </c>
       <c r="BL4" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.227</v>
       </c>
       <c r="BM4" t="n">
-        <v>-0.011</v>
+        <v>-0.012</v>
       </c>
       <c r="BN4" t="n">
-        <v>1.485</v>
+        <v>1.77</v>
       </c>
       <c r="BO4" t="n">
         <v>0</v>
@@ -1608,7 +1608,7 @@
         <v>0</v>
       </c>
       <c r="BQ4" t="n">
-        <v>0.016</v>
+        <v>0.025</v>
       </c>
       <c r="BR4" t="n">
         <v>0</v>
@@ -1617,28 +1617,28 @@
         <v>0</v>
       </c>
       <c r="BT4" t="n">
-        <v>-0.065</v>
+        <v>0.302</v>
       </c>
       <c r="BU4" t="n">
-        <v>-0.028</v>
+        <v>-0.212</v>
       </c>
       <c r="BV4" t="n">
-        <v>0.008</v>
+        <v>0.007</v>
       </c>
       <c r="BW4" t="n">
-        <v>-0.003</v>
+        <v>-0.029</v>
       </c>
       <c r="BX4" t="n">
-        <v>-0.006</v>
+        <v>0.083</v>
       </c>
       <c r="BY4" t="n">
         <v>-0</v>
       </c>
       <c r="BZ4" t="n">
-        <v>-0.006</v>
+        <v>-0.036</v>
       </c>
       <c r="CA4" t="n">
-        <v>0.185</v>
+        <v>0.08</v>
       </c>
       <c r="CB4" t="n">
         <v>-0.002</v>
@@ -1647,25 +1647,25 @@
         <v>-0</v>
       </c>
       <c r="CD4" t="n">
-        <v>-0.001</v>
+        <v>0</v>
       </c>
       <c r="CE4" t="n">
         <v>0</v>
       </c>
       <c r="CF4" t="n">
-        <v>-0.001</v>
+        <v>-0</v>
       </c>
       <c r="CG4" t="n">
         <v>0</v>
       </c>
       <c r="CH4" t="n">
-        <v>1.325</v>
+        <v>0.022</v>
       </c>
       <c r="CI4" t="n">
-        <v>3.3</v>
+        <v>4.398</v>
       </c>
       <c r="CJ4" t="n">
-        <v>479.789</v>
+        <v>409.29</v>
       </c>
     </row>
     <row r="5">
@@ -1673,199 +1673,199 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
+        <v>0.074</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.036</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.415</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.148</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.774</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.122</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="T5" t="n">
+        <v>-0.003</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.513</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.499</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.252</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.628</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>2.224</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>0.392</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>5.29</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>18.261</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.07199999999999999</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.436</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>13.075</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>22.594</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0.774</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>14.658</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>2.274</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>1.954</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.555</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.212</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.355</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>0.335</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="BM5" t="n">
         <v>0.005</v>
       </c>
-      <c r="C5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1.187</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.106</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-0.002</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>2.19</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.105</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-0.001</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.021</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.146</v>
-      </c>
-      <c r="T5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.206</v>
-      </c>
-      <c r="X5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>6.024</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>0.538</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>0.029</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>11.243</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>3.644</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.026</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>0.757</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>-0.001</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0.07199999999999999</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>27.11</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>0.158</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>-0.001</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>17.927</v>
-      </c>
-      <c r="BA5" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>0.073</v>
-      </c>
-      <c r="BC5" t="n">
-        <v>29.537</v>
-      </c>
-      <c r="BD5" t="n">
-        <v>-0.002</v>
-      </c>
-      <c r="BE5" t="n">
-        <v>2.853</v>
-      </c>
-      <c r="BF5" t="n">
-        <v>1.621</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>0.196</v>
-      </c>
-      <c r="BI5" t="n">
-        <v>2.189</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>0.174</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>0.505</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>0.033</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>0.002</v>
-      </c>
       <c r="BN5" t="n">
-        <v>0.757</v>
+        <v>0.727</v>
       </c>
       <c r="BO5" t="n">
         <v>0</v>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
       <c r="BQ5" t="n">
-        <v>0.058</v>
+        <v>0.193</v>
       </c>
       <c r="BR5" t="n">
         <v>0</v>
@@ -1883,55 +1883,55 @@
         <v>0</v>
       </c>
       <c r="BT5" t="n">
-        <v>0.06</v>
+        <v>0.128</v>
       </c>
       <c r="BU5" t="n">
-        <v>0.024</v>
+        <v>0.527</v>
       </c>
       <c r="BV5" t="n">
-        <v>0.002</v>
+        <v>0.083</v>
       </c>
       <c r="BW5" t="n">
-        <v>0.005</v>
+        <v>0.074</v>
       </c>
       <c r="BX5" t="n">
-        <v>0.027</v>
+        <v>0.148</v>
       </c>
       <c r="BY5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="BZ5" t="n">
-        <v>-0.001</v>
+        <v>0.096</v>
       </c>
       <c r="CA5" t="n">
-        <v>0.105</v>
+        <v>0.13</v>
       </c>
       <c r="CB5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CC5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CD5" t="n">
         <v>-0</v>
       </c>
       <c r="CE5" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CF5" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="CG5" t="n">
         <v>0</v>
       </c>
       <c r="CH5" t="n">
-        <v>0.781</v>
+        <v>3.767</v>
       </c>
       <c r="CI5" t="n">
-        <v>1.953</v>
+        <v>1.124</v>
       </c>
       <c r="CJ5" t="n">
-        <v>319.317</v>
+        <v>407.514</v>
       </c>
     </row>
     <row r="6">
@@ -1939,199 +1939,199 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.076</v>
+        <v>0.023</v>
       </c>
       <c r="C6" t="n">
-        <v>0.001</v>
+        <v>-0.004</v>
       </c>
       <c r="D6" t="n">
-        <v>0.003</v>
+        <v>-0.003</v>
       </c>
       <c r="E6" t="n">
-        <v>1.749</v>
+        <v>0.982</v>
       </c>
       <c r="F6" t="n">
-        <v>0.296</v>
+        <v>0.372</v>
       </c>
       <c r="G6" t="n">
-        <v>0.013</v>
+        <v>-0.004</v>
       </c>
       <c r="H6" t="n">
-        <v>0.081</v>
+        <v>0.021</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="K6" t="n">
-        <v>1.612</v>
+        <v>1.748</v>
       </c>
       <c r="L6" t="n">
-        <v>0.362</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="M6" t="n">
-        <v>0.675</v>
+        <v>0.33</v>
       </c>
       <c r="N6" t="n">
-        <v>0.163</v>
+        <v>0.038</v>
       </c>
       <c r="O6" t="n">
-        <v>0.001</v>
+        <v>-0.001</v>
       </c>
       <c r="P6" t="n">
         <v>0</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.002</v>
+        <v>-0.001</v>
       </c>
       <c r="R6" t="n">
-        <v>0.08400000000000001</v>
+        <v>0.073</v>
       </c>
       <c r="S6" t="n">
-        <v>0.307</v>
+        <v>-0.12</v>
       </c>
       <c r="T6" t="n">
-        <v>0.004</v>
+        <v>-0.012</v>
       </c>
       <c r="U6" t="n">
+        <v>-0.007</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="X6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.154</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>4.011</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>2.056</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.198</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>8.304</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>23.589</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>0.032</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>-0.004</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>0.019</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>-0.068</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>0.008999999999999999</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.202</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.136</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>31.967</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="AY6" t="n">
         <v>0.037</v>
       </c>
-      <c r="V6" t="n">
-        <v>0.521</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.706</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0.263</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>5.619</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>1.477</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0.335</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>6.216</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>11.217</v>
-      </c>
-      <c r="AG6" t="n">
-        <v>0.115</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="AL6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AM6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN6" t="n">
-        <v>0.058</v>
-      </c>
-      <c r="AO6" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="AP6" t="n">
-        <v>1.482</v>
-      </c>
-      <c r="AQ6" t="n">
-        <v>0.047</v>
-      </c>
-      <c r="AR6" t="n">
-        <v>-0</v>
-      </c>
-      <c r="AS6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT6" t="n">
-        <v>0.34</v>
-      </c>
-      <c r="AU6" t="n">
-        <v>0.323</v>
-      </c>
-      <c r="AV6" t="n">
-        <v>16.896</v>
-      </c>
-      <c r="AW6" t="n">
-        <v>0.148</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="AY6" t="n">
-        <v>0.163</v>
-      </c>
       <c r="AZ6" t="n">
-        <v>20.323</v>
+        <v>32.151</v>
       </c>
       <c r="BA6" t="n">
-        <v>0.34</v>
+        <v>0.201</v>
       </c>
       <c r="BB6" t="n">
-        <v>0.675</v>
+        <v>0.33</v>
       </c>
       <c r="BC6" t="n">
-        <v>18.92</v>
+        <v>34.039</v>
       </c>
       <c r="BD6" t="n">
-        <v>0.013</v>
+        <v>-0.004</v>
       </c>
       <c r="BE6" t="n">
-        <v>3.795</v>
+        <v>2.589</v>
       </c>
       <c r="BF6" t="n">
-        <v>3.226</v>
+        <v>0.672</v>
       </c>
       <c r="BG6" t="n">
-        <v>0.002</v>
+        <v>-0.005</v>
       </c>
       <c r="BH6" t="n">
-        <v>0.72</v>
+        <v>0.225</v>
       </c>
       <c r="BI6" t="n">
-        <v>1.759</v>
+        <v>1.446</v>
       </c>
       <c r="BJ6" t="n">
-        <v>0.327</v>
+        <v>-0.113</v>
       </c>
       <c r="BK6" t="n">
-        <v>0.703</v>
+        <v>0.55</v>
       </c>
       <c r="BL6" t="n">
-        <v>0.091</v>
+        <v>0.062</v>
       </c>
       <c r="BM6" t="n">
-        <v>0.006</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="BN6" t="n">
-        <v>1.482</v>
+        <v>-0.06900000000000001</v>
       </c>
       <c r="BO6" t="n">
         <v>0</v>
@@ -2140,7 +2140,7 @@
         <v>0</v>
       </c>
       <c r="BQ6" t="n">
-        <v>0.215</v>
+        <v>0.03</v>
       </c>
       <c r="BR6" t="n">
         <v>0</v>
@@ -2149,40 +2149,40 @@
         <v>0</v>
       </c>
       <c r="BT6" t="n">
-        <v>0.214</v>
+        <v>-0.348</v>
       </c>
       <c r="BU6" t="n">
-        <v>0.516</v>
+        <v>0.236</v>
       </c>
       <c r="BV6" t="n">
-        <v>0.065</v>
+        <v>0.038</v>
       </c>
       <c r="BW6" t="n">
-        <v>0.076</v>
+        <v>0.025</v>
       </c>
       <c r="BX6" t="n">
-        <v>0.081</v>
+        <v>0.021</v>
       </c>
       <c r="BY6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="BZ6" t="n">
-        <v>0.091</v>
+        <v>0.024</v>
       </c>
       <c r="CA6" t="n">
-        <v>0.362</v>
+        <v>0.07099999999999999</v>
       </c>
       <c r="CB6" t="n">
-        <v>0</v>
+        <v>-0.002</v>
       </c>
       <c r="CC6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CD6" t="n">
-        <v>0</v>
+        <v>-0.001</v>
       </c>
       <c r="CE6" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="CF6" t="n">
         <v>-0</v>
@@ -2191,13 +2191,13 @@
         <v>0</v>
       </c>
       <c r="CH6" t="n">
-        <v>2.391</v>
+        <v>4.564</v>
       </c>
       <c r="CI6" t="n">
-        <v>1.77</v>
+        <v>0.976</v>
       </c>
       <c r="CJ6" t="n">
-        <v>430.567</v>
+        <v>490.443</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add all updated files
</commit_message>
<xml_diff>
--- a/cluster_center_data.xlsx
+++ b/cluster_center_data.xlsx
@@ -820,160 +820,160 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1.222</v>
+        <v>1.265</v>
       </c>
       <c r="C2" t="n">
-        <v>0.211</v>
+        <v>0.035</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.005</v>
+        <v>0.043</v>
       </c>
       <c r="E2" t="n">
-        <v>-0</v>
+        <v>0.001</v>
       </c>
       <c r="F2" t="n">
-        <v>5.632</v>
+        <v>3.507</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.259</v>
+        <v>1.032</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.005</v>
+        <v>0.202</v>
       </c>
       <c r="I2" t="n">
-        <v>0.068</v>
+        <v>0.046</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.004</v>
+        <v>0.19</v>
       </c>
       <c r="K2" t="n">
-        <v>0.065</v>
+        <v>0.543</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.01</v>
+        <v>0.368</v>
       </c>
       <c r="M2" t="n">
-        <v>0.004</v>
+        <v>0.006</v>
       </c>
       <c r="N2" t="n">
-        <v>0.159</v>
+        <v>0.157</v>
       </c>
       <c r="O2" t="n">
-        <v>-0.005</v>
+        <v>0.011</v>
       </c>
       <c r="P2" t="n">
-        <v>-0.001</v>
+        <v>0.002</v>
       </c>
       <c r="Q2" t="n">
-        <v>-0.014</v>
+        <v>0.134</v>
       </c>
       <c r="R2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="S2" t="n">
-        <v>0.344</v>
+        <v>0.546</v>
       </c>
       <c r="T2" t="n">
-        <v>1.821</v>
+        <v>0.874</v>
       </c>
       <c r="U2" t="n">
-        <v>0.04</v>
+        <v>0.034</v>
       </c>
       <c r="V2" t="n">
-        <v>0.037</v>
+        <v>0.328</v>
       </c>
       <c r="W2" t="n">
-        <v>0.081</v>
+        <v>0.02</v>
       </c>
       <c r="X2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="Z2" t="n">
         <v>0.005</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.02</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="AB2" t="n">
-        <v>1.989</v>
+        <v>2.316</v>
       </c>
       <c r="AC2" t="n">
-        <v>12.618</v>
+        <v>0.678</v>
       </c>
       <c r="AD2" t="n">
-        <v>5.806</v>
+        <v>9.574999999999999</v>
       </c>
       <c r="AE2" t="n">
-        <v>-0.002</v>
+        <v>0.008</v>
       </c>
       <c r="AF2" t="n">
         <v>0</v>
       </c>
       <c r="AG2" t="n">
-        <v>0.031</v>
+        <v>0.035</v>
       </c>
       <c r="AH2" t="n">
-        <v>0.006</v>
+        <v>0.003</v>
       </c>
       <c r="AI2" t="n">
-        <v>0.169</v>
+        <v>0.124</v>
       </c>
       <c r="AJ2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AK2" t="n">
-        <v>25.543</v>
+        <v>12.021</v>
       </c>
       <c r="AL2" t="n">
-        <v>-0.014</v>
+        <v>0.134</v>
       </c>
       <c r="AM2" t="n">
-        <v>20.337</v>
+        <v>13.436</v>
       </c>
       <c r="AN2" t="n">
-        <v>0.037</v>
+        <v>0.328</v>
       </c>
       <c r="AO2" t="n">
-        <v>0.344</v>
+        <v>0.546</v>
       </c>
       <c r="AP2" t="n">
-        <v>26.93</v>
+        <v>13.599</v>
       </c>
       <c r="AQ2" t="n">
-        <v>-0.001</v>
+        <v>0.002</v>
       </c>
       <c r="AR2" t="n">
-        <v>2.352</v>
+        <v>2.325</v>
       </c>
       <c r="AS2" t="n">
-        <v>3.049</v>
+        <v>2.777</v>
       </c>
       <c r="AT2" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AU2" t="n">
-        <v>0.02</v>
+        <v>0.571</v>
       </c>
       <c r="AV2" t="n">
-        <v>1.958</v>
+        <v>1.407</v>
       </c>
       <c r="AW2" t="n">
-        <v>0.23</v>
+        <v>0.178</v>
       </c>
       <c r="AX2" t="n">
-        <v>0.877</v>
+        <v>1.067</v>
       </c>
       <c r="AY2" t="n">
-        <v>0.053</v>
+        <v>-0.007</v>
       </c>
       <c r="AZ2" t="n">
-        <v>-0</v>
+        <v>0.001</v>
       </c>
       <c r="BA2" t="n">
-        <v>1.821</v>
+        <v>0.874</v>
       </c>
       <c r="BB2" t="n">
         <v>0</v>
@@ -982,7 +982,7 @@
         <v>0</v>
       </c>
       <c r="BD2" t="n">
-        <v>0.019</v>
+        <v>0.083</v>
       </c>
       <c r="BE2" t="n">
         <v>0</v>
@@ -991,28 +991,28 @@
         <v>0</v>
       </c>
       <c r="BG2" t="n">
-        <v>0.113</v>
+        <v>0.092</v>
       </c>
       <c r="BH2" t="n">
-        <v>0.022</v>
+        <v>0.465</v>
       </c>
       <c r="BI2" t="n">
-        <v>0.015</v>
+        <v>0.004</v>
       </c>
       <c r="BJ2" t="n">
         <v>0</v>
       </c>
       <c r="BK2" t="n">
-        <v>0.068</v>
+        <v>0.046</v>
       </c>
       <c r="BL2" t="n">
         <v>0</v>
       </c>
       <c r="BM2" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="BN2" t="n">
-        <v>0.02</v>
+        <v>0.5580000000000001</v>
       </c>
       <c r="BO2" t="n">
         <v>0</v>
@@ -1033,19 +1033,19 @@
         <v>0</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.968</v>
+        <v>1.933</v>
       </c>
       <c r="BV2" t="n">
-        <v>2.543</v>
+        <v>0.013</v>
       </c>
       <c r="BW2" t="n">
-        <v>360.344</v>
+        <v>303.396</v>
       </c>
       <c r="BX2" t="n">
-        <v>2.636</v>
+        <v>2.123</v>
       </c>
       <c r="BY2" t="n">
-        <v>3.322</v>
+        <v>2.319</v>
       </c>
     </row>
     <row r="3">
@@ -1053,199 +1053,199 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>1.23</v>
+        <v>1.8</v>
       </c>
       <c r="C3" t="n">
-        <v>0.108</v>
+        <v>0.364</v>
       </c>
       <c r="D3" t="n">
-        <v>0.113</v>
+        <v>0.024</v>
       </c>
       <c r="E3" t="n">
-        <v>0.001</v>
+        <v>-0.001</v>
       </c>
       <c r="F3" t="n">
-        <v>0.36</v>
+        <v>7.642</v>
       </c>
       <c r="G3" t="n">
-        <v>1.832</v>
+        <v>0.47</v>
       </c>
       <c r="H3" t="n">
-        <v>0.18</v>
+        <v>-0.097</v>
       </c>
       <c r="I3" t="n">
-        <v>0.153</v>
+        <v>0.023</v>
       </c>
       <c r="J3" t="n">
-        <v>0.412</v>
+        <v>0.05</v>
       </c>
       <c r="K3" t="n">
-        <v>0.681</v>
+        <v>-0.061</v>
       </c>
       <c r="L3" t="n">
-        <v>0.797</v>
+        <v>0.095</v>
       </c>
       <c r="M3" t="n">
-        <v>0.008</v>
+        <v>-0.001</v>
       </c>
       <c r="N3" t="n">
-        <v>0.307</v>
+        <v>0.148</v>
       </c>
       <c r="O3" t="n">
-        <v>0.024</v>
+        <v>-0.005</v>
       </c>
       <c r="P3" t="n">
-        <v>0.004</v>
+        <v>-0.003</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.235</v>
+        <v>-0.105</v>
       </c>
       <c r="R3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="S3" t="n">
-        <v>1.03</v>
+        <v>-0.173</v>
       </c>
       <c r="T3" t="n">
-        <v>0.879</v>
+        <v>1.317</v>
       </c>
       <c r="U3" t="n">
-        <v>0.063</v>
+        <v>0.006</v>
       </c>
       <c r="V3" t="n">
-        <v>0.478</v>
+        <v>-0.201</v>
       </c>
       <c r="W3" t="n">
-        <v>0.07199999999999999</v>
+        <v>0.046</v>
       </c>
       <c r="X3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Y3" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.01</v>
+        <v>-0.001</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.525</v>
+        <v>-0.219</v>
       </c>
       <c r="AB3" t="n">
-        <v>1.066</v>
+        <v>0.456</v>
       </c>
       <c r="AC3" t="n">
-        <v>1.867</v>
+        <v>18.148</v>
       </c>
       <c r="AD3" t="n">
-        <v>6.473</v>
+        <v>1.216</v>
       </c>
       <c r="AE3" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>0.102</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>34.955</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>-0.105</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>21.98</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>-0.201</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>-0.173</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>36.906</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>-0.003</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>3.431</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>1.471</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>-0.039</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.187</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>1.317</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.029</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>-0.309</v>
+      </c>
+      <c r="BI3" t="n">
         <v>0.007</v>
       </c>
-      <c r="AF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG3" t="n">
-        <v>0.111</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>0.007</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>0.164</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>4.456</v>
-      </c>
-      <c r="AL3" t="n">
-        <v>0.235</v>
-      </c>
-      <c r="AM3" t="n">
-        <v>9.695</v>
-      </c>
-      <c r="AN3" t="n">
-        <v>0.478</v>
-      </c>
-      <c r="AO3" t="n">
-        <v>1.03</v>
-      </c>
-      <c r="AP3" t="n">
-        <v>6.261</v>
-      </c>
-      <c r="AQ3" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="AR3" t="n">
-        <v>2.021</v>
-      </c>
-      <c r="AS3" t="n">
-        <v>2.301</v>
-      </c>
-      <c r="AT3" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="AV3" t="n">
-        <v>0.346</v>
-      </c>
-      <c r="AW3" t="n">
-        <v>0.304</v>
-      </c>
-      <c r="AX3" t="n">
-        <v>0.377</v>
-      </c>
-      <c r="AY3" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="AZ3" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="BA3" t="n">
-        <v>0.879</v>
-      </c>
-      <c r="BB3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD3" t="n">
-        <v>0.159</v>
-      </c>
-      <c r="BE3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>0.193</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>0.717</v>
-      </c>
-      <c r="BI3" t="n">
-        <v>0.014</v>
-      </c>
       <c r="BJ3" t="n">
         <v>0</v>
       </c>
       <c r="BK3" t="n">
-        <v>0.153</v>
+        <v>0.023</v>
       </c>
       <c r="BL3" t="n">
         <v>0</v>
       </c>
       <c r="BM3" t="n">
-        <v>0.019</v>
+        <v>-0.001</v>
       </c>
       <c r="BN3" t="n">
-        <v>0.525</v>
+        <v>-0.219</v>
       </c>
       <c r="BO3" t="n">
         <v>0</v>
@@ -1266,19 +1266,19 @@
         <v>0</v>
       </c>
       <c r="BU3" t="n">
-        <v>1.736</v>
+        <v>0.367</v>
       </c>
       <c r="BV3" t="n">
-        <v>0.038</v>
+        <v>3.418</v>
       </c>
       <c r="BW3" t="n">
-        <v>270.905</v>
+        <v>352.336</v>
       </c>
       <c r="BX3" t="n">
-        <v>2.364</v>
+        <v>2.338</v>
       </c>
       <c r="BY3" t="n">
-        <v>2.416</v>
+        <v>4.402</v>
       </c>
     </row>
     <row r="4">
@@ -1286,70 +1286,70 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>2.424</v>
+        <v>-0.017</v>
       </c>
       <c r="C4" t="n">
-        <v>0.656</v>
+        <v>-0.337</v>
       </c>
       <c r="D4" t="n">
-        <v>0.043</v>
+        <v>-0.032</v>
       </c>
       <c r="E4" t="n">
-        <v>-0</v>
+        <v>0.001</v>
       </c>
       <c r="F4" t="n">
-        <v>8.275</v>
+        <v>0.644</v>
       </c>
       <c r="G4" t="n">
-        <v>0.454</v>
+        <v>-0.404</v>
       </c>
       <c r="H4" t="n">
-        <v>0.003</v>
+        <v>0.264</v>
       </c>
       <c r="I4" t="n">
-        <v>0.08699999999999999</v>
+        <v>-0.117</v>
       </c>
       <c r="J4" t="n">
-        <v>0.215</v>
+        <v>0.036</v>
       </c>
       <c r="K4" t="n">
-        <v>0.191</v>
+        <v>0.653</v>
       </c>
       <c r="L4" t="n">
-        <v>0.401</v>
+        <v>0.074</v>
       </c>
       <c r="M4" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
       <c r="N4" t="n">
-        <v>0.141</v>
+        <v>0.19</v>
       </c>
       <c r="O4" t="n">
-        <v>0.014</v>
+        <v>-0.005</v>
       </c>
       <c r="P4" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.116</v>
+        <v>0.008</v>
       </c>
       <c r="R4" t="n">
         <v>-0</v>
       </c>
       <c r="S4" t="n">
-        <v>0.698</v>
+        <v>-0.366</v>
       </c>
       <c r="T4" t="n">
-        <v>1.514</v>
+        <v>0.6</v>
       </c>
       <c r="U4" t="n">
-        <v>0.047</v>
+        <v>-0.032</v>
       </c>
       <c r="V4" t="n">
-        <v>0.283</v>
+        <v>-0.066</v>
       </c>
       <c r="W4" t="n">
-        <v>0.037</v>
+        <v>0.004</v>
       </c>
       <c r="X4" t="n">
         <v>-0</v>
@@ -1358,88 +1358,88 @@
         <v>-0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.008999999999999999</v>
+        <v>-0.008</v>
       </c>
       <c r="AA4" t="n">
-        <v>-0.011</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="AB4" t="n">
-        <v>-0.44</v>
+        <v>7.832</v>
       </c>
       <c r="AC4" t="n">
-        <v>6.602</v>
+        <v>7.493</v>
       </c>
       <c r="AD4" t="n">
-        <v>1.537</v>
+        <v>6.12</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.012</v>
+        <v>-0.003</v>
       </c>
       <c r="AF4" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="AG4" t="n">
-        <v>0.03</v>
+        <v>0.039</v>
       </c>
       <c r="AH4" t="n">
-        <v>0.002</v>
+        <v>0.006</v>
       </c>
       <c r="AI4" t="n">
-        <v>-0.019</v>
+        <v>0.452</v>
       </c>
       <c r="AJ4" t="n">
         <v>-0</v>
       </c>
       <c r="AK4" t="n">
-        <v>14.53</v>
+        <v>26.169</v>
       </c>
       <c r="AL4" t="n">
-        <v>0.116</v>
+        <v>0.008</v>
       </c>
       <c r="AM4" t="n">
-        <v>12.215</v>
+        <v>16.944</v>
       </c>
       <c r="AN4" t="n">
-        <v>0.283</v>
+        <v>-0.066</v>
       </c>
       <c r="AO4" t="n">
-        <v>0.698</v>
+        <v>-0.366</v>
       </c>
       <c r="AP4" t="n">
-        <v>17.15</v>
+        <v>26.64</v>
       </c>
       <c r="AQ4" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>4.421</v>
+        <v>-0.389</v>
       </c>
       <c r="AS4" t="n">
-        <v>1.384</v>
+        <v>5.717</v>
       </c>
       <c r="AT4" t="n">
         <v>-0</v>
       </c>
       <c r="AU4" t="n">
-        <v>0.317</v>
+        <v>0.49</v>
       </c>
       <c r="AV4" t="n">
-        <v>2.75</v>
+        <v>0.338</v>
       </c>
       <c r="AW4" t="n">
-        <v>0.031</v>
+        <v>0.533</v>
       </c>
       <c r="AX4" t="n">
-        <v>-0.236</v>
+        <v>3.646</v>
       </c>
       <c r="AY4" t="n">
-        <v>0.016</v>
+        <v>0.006</v>
       </c>
       <c r="AZ4" t="n">
-        <v>0.002</v>
+        <v>-0.001</v>
       </c>
       <c r="BA4" t="n">
-        <v>1.514</v>
+        <v>0.6</v>
       </c>
       <c r="BB4" t="n">
         <v>0</v>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
       <c r="BD4" t="n">
-        <v>0.105</v>
+        <v>0.034</v>
       </c>
       <c r="BE4" t="n">
         <v>0</v>
@@ -1457,28 +1457,28 @@
         <v>0</v>
       </c>
       <c r="BG4" t="n">
-        <v>0.052</v>
+        <v>0.225</v>
       </c>
       <c r="BH4" t="n">
-        <v>0.4</v>
+        <v>-0.058</v>
       </c>
       <c r="BI4" t="n">
-        <v>0.006</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="BJ4" t="n">
         <v>0</v>
       </c>
       <c r="BK4" t="n">
-        <v>0.08699999999999999</v>
+        <v>-0.117</v>
       </c>
       <c r="BL4" t="n">
         <v>0</v>
       </c>
       <c r="BM4" t="n">
-        <v>0.018</v>
+        <v>-0.016</v>
       </c>
       <c r="BN4" t="n">
-        <v>-0.011</v>
+        <v>0.8169999999999999</v>
       </c>
       <c r="BO4" t="n">
         <v>0</v>
@@ -1499,19 +1499,19 @@
         <v>0</v>
       </c>
       <c r="BU4" t="n">
-        <v>0.482</v>
+        <v>1.02</v>
       </c>
       <c r="BV4" t="n">
-        <v>1.786</v>
+        <v>1.018</v>
       </c>
       <c r="BW4" t="n">
-        <v>291</v>
+        <v>323.415</v>
       </c>
       <c r="BX4" t="n">
-        <v>1.154</v>
+        <v>1.889</v>
       </c>
       <c r="BY4" t="n">
-        <v>3.082</v>
+        <v>3.242</v>
       </c>
     </row>
     <row r="5">
@@ -1519,160 +1519,160 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.151</v>
+        <v>2.565</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.259</v>
+        <v>0.822</v>
       </c>
       <c r="D5" t="n">
+        <v>-0.019</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="F5" t="n">
+        <v>13.453</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-0.485</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-0.02</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-0.006</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.021</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-0.054</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.004</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="R5" t="n">
         <v>-0</v>
       </c>
-      <c r="E5" t="n">
+      <c r="S5" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="T5" t="n">
+        <v>2.195</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="X5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.007</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>-0.109</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>0.635</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>8.119</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1.113</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>-0.028</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>-0.103</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>22.878</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>0.016</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>15.945</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>0.129</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>25.361</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>5.642</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>2.347</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>-0</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>-0.012</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>4.334</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>-0.111</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0.374</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>-0.003</v>
+      </c>
+      <c r="AZ5" t="n">
         <v>0.001</v>
       </c>
-      <c r="F5" t="n">
-        <v>1.555</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.139</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.192</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.098</v>
-      </c>
-      <c r="J5" t="n">
-        <v>-0.008</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.382</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-0.008</v>
-      </c>
-      <c r="M5" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.193</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-0.003</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0.717</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1.872</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.06900000000000001</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0.285</v>
-      </c>
-      <c r="W5" t="n">
-        <v>0.103</v>
-      </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="AA5" t="n">
-        <v>0.551</v>
-      </c>
-      <c r="AB5" t="n">
-        <v>4.061</v>
-      </c>
-      <c r="AC5" t="n">
-        <v>4.231</v>
-      </c>
-      <c r="AD5" t="n">
-        <v>14.767</v>
-      </c>
-      <c r="AE5" t="n">
-        <v>-0.003</v>
-      </c>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>0.251</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>15.633</v>
-      </c>
-      <c r="AL5" t="n">
-        <v>0.079</v>
-      </c>
-      <c r="AM5" t="n">
-        <v>19.922</v>
-      </c>
-      <c r="AN5" t="n">
-        <v>0.285</v>
-      </c>
-      <c r="AO5" t="n">
-        <v>0.717</v>
-      </c>
-      <c r="AP5" t="n">
-        <v>16.026</v>
-      </c>
-      <c r="AQ5" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="AR5" t="n">
-        <v>0.794</v>
-      </c>
-      <c r="AS5" t="n">
-        <v>4.755</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>0.279</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>0.846</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>0.368</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>1.841</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>0.045</v>
-      </c>
-      <c r="AZ5" t="n">
-        <v>-0</v>
-      </c>
       <c r="BA5" t="n">
-        <v>1.872</v>
+        <v>2.195</v>
       </c>
       <c r="BB5" t="n">
         <v>0</v>
@@ -1681,7 +1681,7 @@
         <v>0</v>
       </c>
       <c r="BD5" t="n">
-        <v>0.002</v>
+        <v>0.024</v>
       </c>
       <c r="BE5" t="n">
         <v>0</v>
@@ -1690,28 +1690,28 @@
         <v>0</v>
       </c>
       <c r="BG5" t="n">
-        <v>0.212</v>
+        <v>-0.006</v>
       </c>
       <c r="BH5" t="n">
-        <v>0.365</v>
+        <v>0.145</v>
       </c>
       <c r="BI5" t="n">
-        <v>0.023</v>
+        <v>-0.001</v>
       </c>
       <c r="BJ5" t="n">
         <v>0</v>
       </c>
       <c r="BK5" t="n">
-        <v>0.098</v>
+        <v>-0.006</v>
       </c>
       <c r="BL5" t="n">
         <v>0</v>
       </c>
       <c r="BM5" t="n">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="BN5" t="n">
-        <v>0.551</v>
+        <v>-0.109</v>
       </c>
       <c r="BO5" t="n">
         <v>0</v>
@@ -1732,19 +1732,19 @@
         <v>0</v>
       </c>
       <c r="BU5" t="n">
-        <v>2.552</v>
+        <v>0.08799999999999999</v>
       </c>
       <c r="BV5" t="n">
-        <v>0.694</v>
+        <v>2.725</v>
       </c>
       <c r="BW5" t="n">
-        <v>381.678</v>
+        <v>344.767</v>
       </c>
       <c r="BX5" t="n">
-        <v>3.584</v>
+        <v>0.472</v>
       </c>
       <c r="BY5" t="n">
-        <v>1.919</v>
+        <v>3.101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>